<commit_message>
Updated batch mode stuff
</commit_message>
<xml_diff>
--- a/Master_Results_File_NEW.xlsx
+++ b/Master_Results_File_NEW.xlsx
@@ -531,44 +531,44 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>01.09.21.50UM.002_PROCESSED.xlsx</t>
+          <t>01.09.21.50UM.003_PROCESSED.xlsx</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>35</v>
       </c>
       <c r="D2" t="n">
-        <v>81.89069676430981</v>
+        <v>68.5745443015133</v>
       </c>
       <c r="E2" t="n">
-        <v>52.80770140718645</v>
+        <v>50.44337779213091</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4743250586274045</v>
+        <v>0.4824206896627805</v>
       </c>
       <c r="G2" t="n">
-        <v>0.000704789715952443</v>
+        <v>0.0007174634465868938</v>
       </c>
       <c r="H2" t="n">
-        <v>-239362.5250544484</v>
+        <v>-247353.7475038553</v>
       </c>
       <c r="I2" t="n">
-        <v>227429.4101527297</v>
+        <v>2280.290147728559</v>
       </c>
       <c r="J2" t="n">
-        <v>4.121677698944244</v>
+        <v>788561.0695067085</v>
       </c>
       <c r="K2" t="n">
-        <v>7.538444877038788</v>
+        <v>7.43478449457637</v>
       </c>
       <c r="L2" t="n">
-        <v>7.512511567301534</v>
+        <v>6.245959085320488</v>
       </c>
       <c r="M2" t="n">
-        <v>-3.384337091098328</v>
+        <v>7.990934214151545</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0001</v>
+        <v>1e-06</v>
       </c>
       <c r="O2" t="n">
         <v>4.500000000000001</v>
@@ -580,7 +580,7 @@
         <v>5.5</v>
       </c>
       <c r="R2" t="n">
-        <v>0.002405775691806065</v>
+        <v>0.001853821505849047</v>
       </c>
       <c r="S2" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Sausage machine now working with some slight quirks
</commit_message>
<xml_diff>
--- a/Master_Results_File_NEW.xlsx
+++ b/Master_Results_File_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,90 +436,95 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>SAMPLE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SALINITY</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TA</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>ORGALK</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>MASS</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>H0</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>X1</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>X2</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>X3</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>pK1</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>pK2</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>pK3</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>CONVERGENCE_FACTOR</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>pK1_INITIAL</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>pK2_INITIAL</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>pK3_INITIAL</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>SSR</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>SELECTED_MINIMISATION</t>
         </is>
@@ -529,60 +534,59 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>01.09.21.50UM.003_PROCESSED.xlsx</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>01.09.21.50UM.001_PROCESSED.xlsx</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>35</v>
       </c>
-      <c r="D2" t="n">
-        <v>68.5745443015133</v>
-      </c>
       <c r="E2" t="n">
-        <v>50.44337779213091</v>
+        <v>83.84526363461985</v>
       </c>
       <c r="F2" t="n">
-        <v>0.4824206896627805</v>
+        <v>55.9456810290643</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0007174634465868938</v>
+        <v>0.4751958900593387</v>
       </c>
       <c r="H2" t="n">
-        <v>-247353.7475038553</v>
+        <v>0.0006988474973753943</v>
       </c>
       <c r="I2" t="n">
-        <v>2280.290147728559</v>
+        <v>49.18227265827269</v>
       </c>
       <c r="J2" t="n">
-        <v>788561.0695067085</v>
+        <v>-0.1185670492652907</v>
       </c>
       <c r="K2" t="n">
-        <v>7.43478449457637</v>
+        <v>206.4969034877071</v>
       </c>
       <c r="L2" t="n">
-        <v>6.245959085320488</v>
-      </c>
-      <c r="M2" t="n">
-        <v>7.990934214151545</v>
-      </c>
+        <v>4.888739345535772</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="n">
-        <v>1e-06</v>
+        <v>10.2018170074276</v>
       </c>
       <c r="O2" t="n">
+        <v>1e-08</v>
+      </c>
+      <c r="P2" t="n">
         <v>4.500000000000001</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>5.250000000000001</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>5.5</v>
       </c>
-      <c r="R2" t="n">
-        <v>0.001853821505849047</v>
-      </c>
       <c r="S2" t="n">
+        <v>0.0009999710533152371</v>
+      </c>
+      <c r="T2" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sausage machine now working with quirks removed
</commit_message>
<xml_diff>
--- a/Master_Results_File_NEW.xlsx
+++ b/Master_Results_File_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,95 +436,100 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SAMPLE</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>SALINITY</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>TA</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ORGALK</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>MASS</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>H0</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>X1</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>X2</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>X3</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>pK1</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>pK2</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>pK3</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>CONVERGENCE_FACTOR</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>pK1_INITIAL</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>pK2_INITIAL</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>pK3_INITIAL</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>SSR</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>SELECTED_MINIMISATION</t>
         </is>
@@ -535,58 +540,59 @@
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
         <is>
           <t>01.09.21.50UM.001_PROCESSED.xlsx</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>35</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>83.84526363461985</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>55.9456810290643</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>0.4751958900593387</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>0.0006988474973753943</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>49.18227265827269</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>-0.1185670492652907</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>206.4969034877071</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>4.888739345535772</v>
       </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="n">
         <v>10.2018170074276</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>1e-08</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>4.500000000000001</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>5.250000000000001</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>5.5</v>
       </c>
-      <c r="S2" t="n">
+      <c r="T2" t="n">
         <v>0.0009999710533152371</v>
       </c>
-      <c r="T2" t="n">
+      <c r="U2" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>